<commit_message>
adjustment in order transaction module
</commit_message>
<xml_diff>
--- a/public/template/order_template.xlsx
+++ b/public/template/order_template.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie Castro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA1CE07-7BFE-4FAD-ACBE-38E7220AA24C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D52879A-607F-48BD-A2E0-BD956CB1D1D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="600" windowWidth="24000" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,78 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Request Time</t>
-  </si>
-  <si>
-    <t>Transaction Number</t>
-  </si>
-  <si>
-    <t>Designation Number</t>
-  </si>
-  <si>
-    <t>No. of Pages</t>
-  </si>
-  <si>
-    <t>Number of Copies</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Middle Initial</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Tel / Mobile number/s</t>
-  </si>
-  <si>
-    <t>House/Building No./Building Name</t>
-  </si>
-  <si>
-    <t>Street Name</t>
-  </si>
-  <si>
-    <t>Barangay</t>
-  </si>
-  <si>
-    <t>City Municipal</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Price</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Payor</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Payment Category</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Email Address</t>
   </si>
   <si>
     <t>Payment Status</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Reference/Transaction/Serial Number</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Department Code</t>
   </si>
 </sst>
 </file>
@@ -114,7 +78,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,14 +104,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,7 +152,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -195,7 +164,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -242,6 +211,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -277,6 +263,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,111 +432,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="75.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>